<commit_message>
Modify first two lessons
</commit_message>
<xml_diff>
--- a/ExcelCo/basics/01_navigation.xlsx
+++ b/ExcelCo/basics/01_navigation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidma/Documents/ExcelCo/basics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidma/Documents/DBC/repos/dma315.github.io/ExcelCo/basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -496,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -620,188 +620,50 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF50A6CE"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF50A6CE"/>
+  <dxfs count="66">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4F5FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4F5FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7D8EC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -897,15 +759,616 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE4F5FD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7D8EC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7D8EC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7D8EC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF969EA7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA7D8EC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF50A6CE"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF50A6CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
+      <color rgb="FFE4F5FD"/>
+      <color rgb="FFA7D8EC"/>
       <color rgb="FF50A6CE"/>
       <color rgb="FF00476A"/>
       <color rgb="FF969EA7"/>
-      <color rgb="FFA7D8EC"/>
-      <color rgb="FFE4F5FD"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1875,35 +2338,40 @@
     <mergeCell ref="B34:N34"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:N8">
-    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="Incomplete">
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",B7)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="24" priority="10" operator="beginsWith" text="Complete">
+    <cfRule type="beginsWith" dxfId="18" priority="13" operator="beginsWith" text="Complete">
       <formula>LEFT(B7,LEN("Complete"))="Complete"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:N19">
-    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="Incomplete">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",B18)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="22" priority="6" operator="beginsWith" text="Complete">
+    <cfRule type="beginsWith" dxfId="16" priority="9" operator="beginsWith" text="Complete">
       <formula>LEFT(B18,LEN("Complete"))="Complete"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:N35">
-    <cfRule type="containsText" dxfId="21" priority="3" operator="containsText" text="Incomplete">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",B34)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="20" priority="4" operator="beginsWith" text="Complete">
+    <cfRule type="beginsWith" dxfId="14" priority="7" operator="beginsWith" text="Complete">
       <formula>LEFT(B34,LEN("Complete"))="Complete"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:N42">
-    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Incomplete">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="Incomplete">
       <formula>NOT(ISERROR(SEARCH("Incomplete",B42)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="2" operator="beginsWith" text="Complete">
+    <cfRule type="beginsWith" dxfId="12" priority="5" operator="beginsWith" text="Complete">
       <formula>LEFT(B42,LEN("Complete"))="Complete"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M5 J13:M13 J24:M24 H40:M40">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="14">
+      <formula>LEN(TRIM(H4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3021,10 +3489,10 @@
       <c r="AY13" s="31"/>
       <c r="AZ13" s="31"/>
       <c r="BA13" s="31"/>
-      <c r="BB13" s="48"/>
-      <c r="BC13" s="49"/>
-      <c r="BD13" s="49"/>
-      <c r="BE13" s="50"/>
+      <c r="BB13" s="55"/>
+      <c r="BC13" s="56"/>
+      <c r="BD13" s="56"/>
+      <c r="BE13" s="57"/>
     </row>
     <row r="14" spans="1:57" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="36"/>
@@ -3669,93 +4137,98 @@
     <mergeCell ref="B2:R2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:Q4">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="65" priority="19" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:R11 R13:R19">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="64" priority="18" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",R5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:Q20">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="63" priority="17" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",E20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D19">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="62" priority="16" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",D7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:O6">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="61" priority="15" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7:P11 P13:P17">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="60" priority="14" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",P7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:O18">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="59" priority="13" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",G18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F17">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="58" priority="12" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",F9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:M8">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="57" priority="11" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:N11 N13:N15">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",N9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16:M16">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="55" priority="9" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:M15">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="54" priority="8" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",I15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H15">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="53" priority="7" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",H11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:K10">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",I10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11 L13">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="51" priority="5" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",L11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BA12">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="50" priority="2" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",K14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="ba">
+    <cfRule type="containsText" dxfId="48" priority="3" operator="containsText" text="ba">
       <formula>NOT(ISERROR(SEARCH("ba",J13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB13">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(BB13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>